<commit_message>
Optimize employer branding sections and update BMQ calculations
- Optimize social media employer branding themes loading (single file read, single-pass processing)
- Remove summary table from employer branding posts section
- Update BMQ calculations to use correct file paths and column names (Headline, URL)
- Update topical analysis to use backlog version for PR topics
- Process and save BMQ results back to agility files
</commit_message>
<xml_diff>
--- a/data/agility/exergi_agility.xlsx
+++ b/data/agility/exergi_agility.xlsx
@@ -7,203 +7,126 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Volume &amp; Quality" sheetId="1" r:id="rId1"/>
-    <sheet name="Sentiment" sheetId="2" r:id="rId2"/>
-    <sheet name="Top Archetypes" sheetId="3" r:id="rId3"/>
-    <sheet name="Key Topics" sheetId="4" r:id="rId4"/>
-    <sheet name="Topics per Archetype" sheetId="5" r:id="rId5"/>
-    <sheet name="Raw Data" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="158">
-  <si>
-    <t>Volume</t>
-  </si>
-  <si>
-    <t>16/100</t>
-  </si>
-  <si>
-    <t>Negative</t>
-  </si>
-  <si>
-    <t>Neutral</t>
-  </si>
-  <si>
-    <t>Positive</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="161">
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Media Outlet</t>
+  </si>
+  <si>
+    <t>Published</t>
+  </si>
+  <si>
+    <t>Snippet</t>
+  </si>
+  <si>
+    <t>UVM (Insights by Similarweb)</t>
+  </si>
+  <si>
+    <t>Journalist Shares</t>
+  </si>
+  <si>
+    <t>Journalist Reach</t>
+  </si>
+  <si>
+    <t>Total Engagement</t>
+  </si>
+  <si>
+    <t>Sentiment</t>
+  </si>
+  <si>
+    <t>Media Outlet City</t>
+  </si>
+  <si>
+    <t>Media Outlet Region</t>
+  </si>
+  <si>
+    <t>Media Outlet Country</t>
+  </si>
+  <si>
+    <t>Advertising Value Equivalency</t>
+  </si>
+  <si>
+    <t>Domain Authority (provided by Moz)</t>
+  </si>
+  <si>
+    <t>Pitch Placement</t>
+  </si>
+  <si>
+    <t>Headline</t>
+  </si>
+  <si>
+    <t>Outlet</t>
+  </si>
+  <si>
+    <t>Published Date</t>
+  </si>
+  <si>
+    <t>Contextual Snippet</t>
+  </si>
+  <si>
+    <t>Impressions</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>AVE(USD)</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>Maintext</t>
+  </si>
+  <si>
+    <t>Publication_Date</t>
+  </si>
+  <si>
+    <t>Full_Title</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>Topics_Sentiments</t>
+  </si>
+  <si>
+    <t>Topic 1</t>
+  </si>
+  <si>
+    <t>Sentiment 1</t>
+  </si>
+  <si>
+    <t>Topic 2</t>
+  </si>
+  <si>
+    <t>Sentiment 2</t>
+  </si>
+  <si>
+    <t>Topic 3</t>
+  </si>
+  <si>
+    <t>Sentiment 3</t>
   </si>
   <si>
     <t>Top Archetype</t>
   </si>
   <si>
-    <t>Count</t>
-  </si>
-  <si>
-    <t>Percentage</t>
-  </si>
-  <si>
-    <t>The Eco Warrior</t>
-  </si>
-  <si>
-    <t>The Value-Seeker</t>
-  </si>
-  <si>
-    <t>Parsing Error</t>
-  </si>
-  <si>
-    <t>The Technologist</t>
-  </si>
-  <si>
-    <t>The Expert</t>
-  </si>
-  <si>
-    <t>Topic Cluster</t>
-  </si>
-  <si>
-    <t>No Topic</t>
-  </si>
-  <si>
-    <t>Financial Performance and Revenue</t>
-  </si>
-  <si>
-    <t>Sustainability and Environmental Innovation</t>
-  </si>
-  <si>
-    <t>Collaboration and Partnerships</t>
-  </si>
-  <si>
-    <t>Carbon Capture and Storage (CCS) Technology</t>
-  </si>
-  <si>
-    <t>Waste Management and Recycling Systems</t>
-  </si>
-  <si>
-    <t>Financial Outlook and Investment Strategies</t>
-  </si>
-  <si>
-    <t>Technological Development and Implementation</t>
-  </si>
-  <si>
-    <t>Climate Change Mitigation Strategies</t>
-  </si>
-  <si>
-    <t>Energy Transition and Climate Benefits</t>
-  </si>
-  <si>
-    <t>Archetype</t>
-  </si>
-  <si>
-    <t>Article</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
-    <t>Media Outlet</t>
-  </si>
-  <si>
-    <t>Published</t>
-  </si>
-  <si>
-    <t>Snippet</t>
-  </si>
-  <si>
-    <t>UVM (Insights by Similarweb)</t>
-  </si>
-  <si>
-    <t>Journalist Shares</t>
-  </si>
-  <si>
-    <t>Journalist Reach</t>
-  </si>
-  <si>
-    <t>Total Engagement</t>
-  </si>
-  <si>
-    <t>Sentiment</t>
-  </si>
-  <si>
-    <t>Media Outlet City</t>
-  </si>
-  <si>
-    <t>Media Outlet Region</t>
-  </si>
-  <si>
-    <t>Media Outlet Country</t>
-  </si>
-  <si>
-    <t>Advertising Value Equivalency</t>
-  </si>
-  <si>
-    <t>Domain Authority (provided by Moz)</t>
-  </si>
-  <si>
-    <t>Pitch Placement</t>
-  </si>
-  <si>
-    <t>Headline</t>
-  </si>
-  <si>
-    <t>Outlet</t>
-  </si>
-  <si>
-    <t>Published Date</t>
-  </si>
-  <si>
-    <t>Contextual Snippet</t>
-  </si>
-  <si>
-    <t>Impressions</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>AVE(USD)</t>
-  </si>
-  <si>
-    <t>company</t>
-  </si>
-  <si>
-    <t>Maintext</t>
-  </si>
-  <si>
-    <t>Publication_Date</t>
-  </si>
-  <si>
-    <t>Full_Title</t>
-  </si>
-  <si>
-    <t>content</t>
-  </si>
-  <si>
-    <t>Topics_Sentiments</t>
-  </si>
-  <si>
-    <t>Topic 1</t>
-  </si>
-  <si>
-    <t>Sentiment 1</t>
-  </si>
-  <si>
-    <t>Topic 2</t>
-  </si>
-  <si>
-    <t>Sentiment 2</t>
-  </si>
-  <si>
-    <t>Topic 3</t>
-  </si>
-  <si>
-    <t>Sentiment 3</t>
-  </si>
-  <si>
     <t>Cluster_Topic2</t>
   </si>
   <si>
@@ -211,6 +134,33 @@
   </si>
   <si>
     <t>Cluster_Topic3</t>
+  </si>
+  <si>
+    <t>query_occurrences</t>
+  </si>
+  <si>
+    <t>term_in_truncated_maintext_100</t>
+  </si>
+  <si>
+    <t>term_in_truncated_maintext_200</t>
+  </si>
+  <si>
+    <t>term_in_title</t>
+  </si>
+  <si>
+    <t>Quality</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Log_Rank</t>
+  </si>
+  <si>
+    <t>Quality_Score</t>
+  </si>
+  <si>
+    <t>BMQ</t>
   </si>
   <si>
     <t>Cramo först in och sist ut när Beccs Stockholm växer fram</t>
@@ -412,6 +362,15 @@
   </si>
   <si>
     <t>One is with a Yara ammonia plant in the Netherlands, another with two of Ørsted's biofuel plants in Denmark, and the third with a Stockholm Exergi thermal power plant in Sweden.</t>
+  </si>
+  <si>
+    <t>Neutral</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Negative</t>
   </si>
   <si>
     <t>Stockholm</t>
@@ -762,9 +721,6 @@
     <t>KTH leder nytt centrum för fossilfri kemikalieproduktion</t>
   </si>
   <si>
-    <t>nan</t>
-  </si>
-  <si>
     <t>It seems there was no news article provided. Please share a news article or its content, and I will extract the key topics and assess their sentiment for you.</t>
   </si>
   <si>
@@ -849,6 +805,54 @@
 Sentiment 2: Neutral  
 Topic 3: Financial Viability of CCS  
 Sentiment 3: Negative  </t>
+  </si>
+  <si>
+    <t>Parsing Error</t>
+  </si>
+  <si>
+    <t>The Technologist</t>
+  </si>
+  <si>
+    <t>The Eco Warrior</t>
+  </si>
+  <si>
+    <t>The Value-Seeker</t>
+  </si>
+  <si>
+    <t>The Expert</t>
+  </si>
+  <si>
+    <t>No Topic</t>
+  </si>
+  <si>
+    <t>Technological Development and Implementation</t>
+  </si>
+  <si>
+    <t>Waste Management and Recycling Systems</t>
+  </si>
+  <si>
+    <t>Carbon Capture and Storage (CCS) Technology</t>
+  </si>
+  <si>
+    <t>Sustainability and Environmental Innovation</t>
+  </si>
+  <si>
+    <t>Collaboration and Partnerships</t>
+  </si>
+  <si>
+    <t>Financial Performance and Revenue</t>
+  </si>
+  <si>
+    <t>Climate Change Mitigation Strategies</t>
+  </si>
+  <si>
+    <t>Energy Transition and Climate Benefits</t>
+  </si>
+  <si>
+    <t>Financial Outlook and Investment Strategies</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -1223,550 +1227,194 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:AW17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:49">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:49">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>6.2</v>
-      </c>
-      <c r="B2">
-        <v>31.2</v>
-      </c>
-      <c r="C2">
-        <v>62.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>43.8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>18.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>6.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>6.2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2">
-        <v>18.8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3">
-        <v>18.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4">
-        <v>16.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5">
-        <v>10.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6">
-        <v>10.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7">
-        <v>8.300000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8">
-        <v>6.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11">
-        <v>2.1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2">
-        <v>100</v>
+        <v>49</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3">
-        <v>33.3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4">
-        <v>33.3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5">
-        <v>33.3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6">
-        <v>23.8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9">
-        <v>50</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10">
-        <v>33.3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11">
-        <v>16.7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>100</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AN17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:40">
-      <c r="A1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:40">
-      <c r="A2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="E2" s="3">
         <v>45943.08333333334</v>
       </c>
       <c r="F2" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="G2">
         <v>588967</v>
       </c>
       <c r="K2" t="s">
-        <v>3</v>
+        <v>109</v>
       </c>
       <c r="L2" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="M2" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="N2" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="O2">
         <v>5447.94</v>
@@ -1775,66 +1423,90 @@
         <v>89</v>
       </c>
       <c r="R2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="S2" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="T2" s="3">
         <v>45943</v>
       </c>
       <c r="U2" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="V2">
         <v>588967</v>
       </c>
       <c r="W2" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="X2">
         <v>5447.94</v>
       </c>
       <c r="Y2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AC2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK2" t="s">
         <v>145</v>
       </c>
-      <c r="AD2" t="s">
-        <v>146</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>10</v>
-      </c>
       <c r="AL2" t="s">
-        <v>14</v>
+        <v>150</v>
       </c>
       <c r="AM2" t="s">
-        <v>14</v>
+        <v>150</v>
       </c>
       <c r="AN2" t="s">
-        <v>14</v>
+        <v>150</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AT2">
+        <v>9270</v>
+      </c>
+      <c r="AU2">
+        <v>1</v>
+      </c>
+      <c r="AV2">
+        <v>0</v>
+      </c>
+      <c r="AW2">
+        <v>0.3760287583079845</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:49">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="E3" s="3">
         <v>45951.08333333334</v>
       </c>
       <c r="F3" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="G3">
         <v>588967</v>
@@ -1849,16 +1521,16 @@
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="L3" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="M3" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="N3" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="O3">
         <v>5447.94</v>
@@ -1867,84 +1539,111 @@
         <v>89</v>
       </c>
       <c r="R3" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="S3" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="T3" s="3">
         <v>45951</v>
       </c>
       <c r="U3" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="V3">
         <v>588967</v>
       </c>
       <c r="W3" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="X3">
         <v>5447.94</v>
       </c>
       <c r="Y3" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="Z3" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="AA3" s="3">
         <v>45951.33333333334</v>
       </c>
       <c r="AB3" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="AC3" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="AD3" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="AF3" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="AH3" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="AJ3" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="AK3" t="s">
-        <v>11</v>
+        <v>146</v>
       </c>
       <c r="AL3" t="s">
-        <v>21</v>
+        <v>151</v>
       </c>
       <c r="AM3" t="s">
-        <v>17</v>
+        <v>155</v>
       </c>
       <c r="AN3" t="s">
-        <v>23</v>
+        <v>158</v>
+      </c>
+      <c r="AO3">
+        <v>5</v>
+      </c>
+      <c r="AP3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>160</v>
+      </c>
+      <c r="AT3">
+        <v>9270</v>
+      </c>
+      <c r="AU3">
+        <v>0.8498</v>
+      </c>
+      <c r="AV3">
+        <v>2</v>
+      </c>
+      <c r="AW3">
+        <v>0.6193281196675693</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:49">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="E4" s="3">
         <v>45939.0625</v>
       </c>
       <c r="F4" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="G4">
         <v>588967</v>
@@ -1959,16 +1658,16 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="L4" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="M4" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="N4" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="O4">
         <v>5447.94</v>
@@ -1977,96 +1676,123 @@
         <v>89</v>
       </c>
       <c r="R4" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="S4" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="T4" s="3">
         <v>45939</v>
       </c>
       <c r="U4" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="V4">
         <v>588967</v>
       </c>
       <c r="W4" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="X4">
         <v>5447.94</v>
       </c>
       <c r="Y4" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="Z4" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="AA4" s="3">
         <v>45939.3125</v>
       </c>
       <c r="AB4" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="AC4" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="AD4" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="AF4" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="AH4" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="AJ4" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="AK4" t="s">
-        <v>8</v>
+        <v>147</v>
       </c>
       <c r="AL4" t="s">
-        <v>19</v>
+        <v>152</v>
       </c>
       <c r="AM4" t="s">
-        <v>16</v>
+        <v>154</v>
       </c>
       <c r="AN4" t="s">
-        <v>21</v>
+        <v>151</v>
+      </c>
+      <c r="AO4">
+        <v>1</v>
+      </c>
+      <c r="AP4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>160</v>
+      </c>
+      <c r="AT4">
+        <v>9270</v>
+      </c>
+      <c r="AU4">
+        <v>0.762</v>
+      </c>
+      <c r="AV4">
+        <v>0</v>
+      </c>
+      <c r="AW4">
+        <v>0.3760287583079845</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:49">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="E5" s="3">
         <v>45908.48436342592</v>
       </c>
       <c r="F5" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="G5">
         <v>2285700</v>
       </c>
       <c r="K5" t="s">
-        <v>2</v>
+        <v>111</v>
       </c>
       <c r="L5" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="N5" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="O5">
         <v>21142.72</v>
@@ -2075,99 +1801,126 @@
         <v>89</v>
       </c>
       <c r="R5" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="S5" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="T5" s="3">
         <v>45908</v>
       </c>
       <c r="U5" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="V5">
         <v>2285700</v>
       </c>
       <c r="W5" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="X5">
         <v>21142.72</v>
       </c>
       <c r="Y5" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="Z5" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="AA5" s="3">
         <v>45908.64892361111</v>
       </c>
       <c r="AB5" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="AC5" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="AD5" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="AF5" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>111</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>110</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>153</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>154</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>159</v>
+      </c>
+      <c r="AO5">
+        <v>1</v>
+      </c>
+      <c r="AP5" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ5" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>160</v>
+      </c>
+      <c r="AT5">
+        <v>8941</v>
+      </c>
+      <c r="AU5">
+        <v>0.6995999999999999</v>
+      </c>
+      <c r="AV5">
         <v>2</v>
       </c>
-      <c r="AH5" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>4</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>16</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>20</v>
+      <c r="AW5">
+        <v>0.5015191845349909</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:49">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="D6" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="E6" s="3">
         <v>45910.14776620371</v>
       </c>
       <c r="F6" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="G6">
         <v>1769848</v>
       </c>
       <c r="K6" t="s">
-        <v>3</v>
+        <v>109</v>
       </c>
       <c r="L6" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="M6" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="N6" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="O6">
         <v>16371.09</v>
@@ -2176,69 +1929,93 @@
         <v>79</v>
       </c>
       <c r="R6" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="S6" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="T6" s="3">
         <v>45910</v>
       </c>
       <c r="U6" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="V6">
         <v>1769848</v>
       </c>
       <c r="W6" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="X6">
         <v>16371.09</v>
       </c>
       <c r="Y6" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="AA6" s="3">
         <v>45910.39491898148</v>
       </c>
       <c r="AB6" t="s">
-        <v>143</v>
-      </c>
-      <c r="AC6" t="s">
+        <v>131</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>137</v>
+      </c>
+      <c r="AK6" t="s">
         <v>145</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AL6" t="s">
         <v>150</v>
       </c>
-      <c r="AK6" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>14</v>
-      </c>
       <c r="AM6" t="s">
-        <v>14</v>
+        <v>150</v>
       </c>
       <c r="AN6" t="s">
-        <v>14</v>
+        <v>150</v>
+      </c>
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>160</v>
+      </c>
+      <c r="AT6">
+        <v>9583</v>
+      </c>
+      <c r="AU6">
+        <v>0.6513</v>
+      </c>
+      <c r="AV6">
+        <v>0</v>
+      </c>
+      <c r="AW6">
+        <v>0.3755780784953673</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:49">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="E7" s="3">
         <v>45908</v>
       </c>
       <c r="F7" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="G7">
         <v>1098249</v>
@@ -2253,13 +2030,13 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>3</v>
+        <v>109</v>
       </c>
       <c r="L7" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="N7" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="O7">
         <v>10158.8</v>
@@ -2268,78 +2045,105 @@
         <v>70</v>
       </c>
       <c r="R7" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="S7" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="T7" s="3">
         <v>45908</v>
       </c>
       <c r="U7" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="V7">
         <v>1098249</v>
       </c>
       <c r="W7" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="X7">
         <v>10158.8</v>
       </c>
       <c r="Y7" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="Z7" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="AB7" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="AC7" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="AD7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="AF7" t="s">
-        <v>3</v>
+        <v>109</v>
       </c>
       <c r="AH7" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="AJ7" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="AK7" t="s">
-        <v>9</v>
+        <v>148</v>
       </c>
       <c r="AL7" t="s">
-        <v>16</v>
+        <v>154</v>
       </c>
       <c r="AM7" t="s">
-        <v>16</v>
+        <v>154</v>
       </c>
       <c r="AN7" t="s">
-        <v>17</v>
+        <v>155</v>
+      </c>
+      <c r="AO7">
+        <v>0</v>
+      </c>
+      <c r="AP7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>160</v>
+      </c>
+      <c r="AT7">
+        <v>9130</v>
+      </c>
+      <c r="AU7">
+        <v>0.6118</v>
+      </c>
+      <c r="AV7">
+        <v>0</v>
+      </c>
+      <c r="AW7">
+        <v>0.3762352882020532</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:49">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="E8" s="3">
         <v>45905.20196759259</v>
       </c>
       <c r="F8" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="G8">
         <v>3773492</v>
@@ -2354,16 +2158,16 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="L8" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="M8" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="N8" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="O8">
         <v>34904.8</v>
@@ -2372,81 +2176,108 @@
         <v>84</v>
       </c>
       <c r="R8" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="S8" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="T8" s="3">
         <v>45905</v>
       </c>
       <c r="U8" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="V8">
         <v>3773492</v>
       </c>
       <c r="W8" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="X8">
         <v>34904.8</v>
       </c>
       <c r="Y8" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="Z8" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="AA8" s="3">
         <v>45905.45196759259</v>
       </c>
       <c r="AB8" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="AC8" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="AD8" t="s">
+        <v>139</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>147</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>154</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>157</v>
+      </c>
+      <c r="AN8" t="s">
         <v>152</v>
       </c>
-      <c r="AF8" t="s">
-        <v>4</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>4</v>
-      </c>
-      <c r="AK8" t="s">
-        <v>8</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>16</v>
-      </c>
-      <c r="AM8" t="s">
-        <v>22</v>
-      </c>
-      <c r="AN8" t="s">
-        <v>19</v>
+      <c r="AO8">
+        <v>0</v>
+      </c>
+      <c r="AP8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>160</v>
+      </c>
+      <c r="AT8">
+        <v>3300</v>
+      </c>
+      <c r="AU8">
+        <v>0.5784</v>
+      </c>
+      <c r="AV8">
+        <v>0</v>
+      </c>
+      <c r="AW8">
+        <v>0.390046439378816</v>
       </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:49">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="E9" s="3">
         <v>45903</v>
       </c>
       <c r="F9" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="G9">
         <v>562175</v>
@@ -2461,10 +2292,10 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="N9" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="O9">
         <v>5200.12</v>
@@ -2473,96 +2304,123 @@
         <v>75</v>
       </c>
       <c r="R9" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="S9" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="T9" s="3">
         <v>45903</v>
       </c>
       <c r="U9" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="V9">
         <v>562175</v>
       </c>
       <c r="W9" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="X9">
         <v>5200.12</v>
       </c>
       <c r="Y9" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="Z9" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="AA9" s="3">
         <v>45973</v>
       </c>
       <c r="AB9" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="AC9" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="AD9" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>110</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>110</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>110</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>147</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>155</v>
+      </c>
+      <c r="AM9" t="s">
         <v>153</v>
       </c>
-      <c r="AF9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ9" t="s">
-        <v>4</v>
-      </c>
-      <c r="AK9" t="s">
-        <v>8</v>
-      </c>
-      <c r="AL9" t="s">
-        <v>17</v>
-      </c>
-      <c r="AM9" t="s">
-        <v>18</v>
-      </c>
       <c r="AN9" t="s">
-        <v>20</v>
+        <v>159</v>
+      </c>
+      <c r="AO9">
+        <v>0</v>
+      </c>
+      <c r="AP9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>160</v>
+      </c>
+      <c r="AT9">
+        <v>12526</v>
+      </c>
+      <c r="AU9">
+        <v>0.5494</v>
+      </c>
+      <c r="AV9">
+        <v>0</v>
+      </c>
+      <c r="AW9">
+        <v>0.3719433622698347</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:49">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="D10" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="E10" s="3">
         <v>45897.23893518518</v>
       </c>
       <c r="F10" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="G10">
         <v>778729</v>
       </c>
       <c r="K10" t="s">
-        <v>3</v>
+        <v>109</v>
       </c>
       <c r="M10" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="N10" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="O10">
         <v>7203.24</v>
@@ -2571,63 +2429,87 @@
         <v>68</v>
       </c>
       <c r="R10" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="S10" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="T10" s="3">
         <v>45897</v>
       </c>
       <c r="U10" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="V10">
         <v>778729</v>
       </c>
       <c r="W10" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="X10">
         <v>7203.24</v>
       </c>
       <c r="Y10" t="s">
-        <v>130</v>
-      </c>
-      <c r="AC10" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK10" t="s">
         <v>145</v>
       </c>
-      <c r="AD10" t="s">
-        <v>146</v>
-      </c>
-      <c r="AK10" t="s">
-        <v>10</v>
-      </c>
       <c r="AL10" t="s">
-        <v>14</v>
+        <v>150</v>
       </c>
       <c r="AM10" t="s">
-        <v>14</v>
+        <v>150</v>
       </c>
       <c r="AN10" t="s">
-        <v>14</v>
+        <v>150</v>
+      </c>
+      <c r="AO10">
+        <v>0</v>
+      </c>
+      <c r="AP10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS10" t="s">
+        <v>160</v>
+      </c>
+      <c r="AT10">
+        <v>50866</v>
+      </c>
+      <c r="AU10">
+        <v>0.5239</v>
+      </c>
+      <c r="AV10">
+        <v>0</v>
+      </c>
+      <c r="AW10">
+        <v>0.3529241379084694</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:49">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="D11" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="E11" s="3">
         <v>45898</v>
       </c>
       <c r="F11" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="G11">
         <v>1098249</v>
@@ -2642,13 +2524,13 @@
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>3</v>
+        <v>109</v>
       </c>
       <c r="L11" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="N11" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="O11">
         <v>10158.8</v>
@@ -2657,90 +2539,117 @@
         <v>70</v>
       </c>
       <c r="R11" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="S11" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="T11" s="3">
         <v>45898</v>
       </c>
       <c r="U11" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="V11">
         <v>1098249</v>
       </c>
       <c r="W11" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="X11">
         <v>10158.8</v>
       </c>
       <c r="Y11" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="Z11" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="AB11" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="AC11" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="AD11" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="AF11" t="s">
-        <v>3</v>
+        <v>109</v>
       </c>
       <c r="AH11" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="AJ11" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="AK11" t="s">
-        <v>9</v>
+        <v>148</v>
       </c>
       <c r="AL11" t="s">
-        <v>16</v>
+        <v>154</v>
       </c>
       <c r="AM11" t="s">
-        <v>16</v>
+        <v>154</v>
       </c>
       <c r="AN11" t="s">
-        <v>17</v>
+        <v>155</v>
+      </c>
+      <c r="AO11">
+        <v>0</v>
+      </c>
+      <c r="AP11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS11" t="s">
+        <v>160</v>
+      </c>
+      <c r="AT11">
+        <v>9130</v>
+      </c>
+      <c r="AU11">
+        <v>0.5011</v>
+      </c>
+      <c r="AV11">
+        <v>0</v>
+      </c>
+      <c r="AW11">
+        <v>0.3762352882020532</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:49">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="E12" s="3">
         <v>45897.24021990741</v>
       </c>
       <c r="F12" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="G12">
         <v>1191791</v>
       </c>
       <c r="K12" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="M12" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="N12" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="O12">
         <v>11024.07</v>
@@ -2749,90 +2658,117 @@
         <v>69</v>
       </c>
       <c r="R12" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="S12" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="T12" s="3">
         <v>45897</v>
       </c>
       <c r="U12" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="V12">
         <v>1191791</v>
       </c>
       <c r="W12" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="X12">
         <v>11024.07</v>
       </c>
       <c r="Y12" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="Z12" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="AA12" s="3">
         <v>45897.40509259259</v>
       </c>
       <c r="AB12" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>141</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>110</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>110</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>111</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>149</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>156</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>156</v>
+      </c>
+      <c r="AN12" t="s">
+        <v>156</v>
+      </c>
+      <c r="AO12">
+        <v>1</v>
+      </c>
+      <c r="AP12" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ12" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS12" t="s">
+        <v>160</v>
+      </c>
+      <c r="AT12">
+        <v>34677</v>
+      </c>
+      <c r="AU12">
+        <v>0.4804</v>
+      </c>
+      <c r="AV12">
+        <v>2</v>
+      </c>
+      <c r="AW12">
+        <v>0.4831237025483648</v>
+      </c>
+    </row>
+    <row r="13" spans="1:49">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="AC12" t="s">
-        <v>137</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>154</v>
-      </c>
-      <c r="AF12" t="s">
-        <v>4</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ12" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK12" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL12" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM12" t="s">
-        <v>15</v>
-      </c>
-      <c r="AN12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:40">
-      <c r="A13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="D13" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="E13" s="3">
         <v>45897.23851851852</v>
       </c>
       <c r="F13" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="G13">
         <v>4648460</v>
       </c>
       <c r="K13" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="N13" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="O13">
         <v>42998.26</v>
@@ -2841,81 +2777,108 @@
         <v>90</v>
       </c>
       <c r="R13" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="S13" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="T13" s="3">
         <v>45897</v>
       </c>
       <c r="U13" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="V13">
         <v>4648460</v>
       </c>
       <c r="W13" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="X13">
         <v>42998.26</v>
       </c>
       <c r="Y13" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="Z13" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="AA13" s="3">
         <v>45897.40518518518</v>
       </c>
       <c r="AB13" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="AC13" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="AD13" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="AF13" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="AH13" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="AJ13" t="s">
+        <v>111</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>148</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>156</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>156</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>156</v>
+      </c>
+      <c r="AO13">
+        <v>1</v>
+      </c>
+      <c r="AP13" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ13" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR13" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS13" t="s">
+        <v>160</v>
+      </c>
+      <c r="AT13">
+        <v>14771</v>
+      </c>
+      <c r="AU13">
+        <v>0.4616</v>
+      </c>
+      <c r="AV13">
         <v>2</v>
       </c>
-      <c r="AK13" t="s">
-        <v>9</v>
-      </c>
-      <c r="AL13" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM13" t="s">
-        <v>15</v>
-      </c>
-      <c r="AN13" t="s">
-        <v>15</v>
+      <c r="AW13">
+        <v>0.4947059406831031</v>
       </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:49">
       <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="D14" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="E14" s="3">
         <v>45897.18328703703</v>
       </c>
       <c r="F14" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="G14">
         <v>3773492</v>
@@ -2930,16 +2893,16 @@
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="L14" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="M14" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="N14" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="O14">
         <v>34904.8</v>
@@ -2948,81 +2911,108 @@
         <v>84</v>
       </c>
       <c r="R14" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="S14" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="T14" s="3">
         <v>45897</v>
       </c>
       <c r="U14" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="V14">
         <v>3773492</v>
       </c>
       <c r="W14" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="X14">
         <v>34904.8</v>
       </c>
       <c r="Y14" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="Z14" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="AA14" s="3">
         <v>45897.43328703703</v>
       </c>
       <c r="AB14" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="AC14" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="AD14" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="AF14" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="AH14" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="AJ14" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="AK14" t="s">
-        <v>8</v>
+        <v>147</v>
       </c>
       <c r="AL14" t="s">
-        <v>16</v>
+        <v>154</v>
       </c>
       <c r="AM14" t="s">
-        <v>19</v>
+        <v>152</v>
       </c>
       <c r="AN14" t="s">
-        <v>19</v>
+        <v>152</v>
+      </c>
+      <c r="AO14">
+        <v>0</v>
+      </c>
+      <c r="AP14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS14" t="s">
+        <v>160</v>
+      </c>
+      <c r="AT14">
+        <v>3300</v>
+      </c>
+      <c r="AU14">
+        <v>0.4442</v>
+      </c>
+      <c r="AV14">
+        <v>0</v>
+      </c>
+      <c r="AW14">
+        <v>0.390046439378816</v>
       </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:49">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="D15" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="E15" s="3">
         <v>45897.23837962963</v>
       </c>
       <c r="F15" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="G15">
         <v>1594618</v>
@@ -3037,13 +3027,13 @@
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="L15" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="N15" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="O15">
         <v>14750.22</v>
@@ -3052,84 +3042,111 @@
         <v>78</v>
       </c>
       <c r="R15" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="S15" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="T15" s="3">
         <v>45897</v>
       </c>
       <c r="U15" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="V15">
         <v>1594618</v>
       </c>
       <c r="W15" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="X15">
         <v>14750.22</v>
       </c>
       <c r="Y15" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="Z15" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="AA15" s="3">
         <v>45897.4050462963</v>
       </c>
       <c r="AB15" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="AC15" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="AD15" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="AF15" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="AH15" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="AJ15" t="s">
+        <v>111</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>148</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>156</v>
+      </c>
+      <c r="AM15" t="s">
+        <v>156</v>
+      </c>
+      <c r="AN15" t="s">
+        <v>156</v>
+      </c>
+      <c r="AO15">
+        <v>1</v>
+      </c>
+      <c r="AP15" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ15" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR15" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS15" t="s">
+        <v>160</v>
+      </c>
+      <c r="AT15">
+        <v>18918</v>
+      </c>
+      <c r="AU15">
+        <v>0.4282</v>
+      </c>
+      <c r="AV15">
         <v>2</v>
       </c>
-      <c r="AK15" t="s">
-        <v>9</v>
-      </c>
-      <c r="AL15" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM15" t="s">
-        <v>15</v>
-      </c>
-      <c r="AN15" t="s">
-        <v>15</v>
+      <c r="AW15">
+        <v>0.4913476493396391</v>
       </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:49">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="E16" s="3">
         <v>45892.46414351852</v>
       </c>
       <c r="F16" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="G16">
         <v>2285700</v>
@@ -3144,13 +3161,13 @@
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="L16" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="N16" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="O16">
         <v>21142.72</v>
@@ -3159,81 +3176,108 @@
         <v>89</v>
       </c>
       <c r="R16" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="S16" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="T16" s="3">
         <v>45892</v>
       </c>
       <c r="U16" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="V16">
         <v>2285700</v>
       </c>
       <c r="W16" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="X16">
         <v>21142.72</v>
       </c>
       <c r="Y16" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="Z16" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="AA16" s="3">
         <v>45892.62331018518</v>
       </c>
       <c r="AB16" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="AC16" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="AD16" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="AF16" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="AH16" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="AJ16" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="AK16" t="s">
-        <v>8</v>
+        <v>147</v>
       </c>
       <c r="AL16" t="s">
-        <v>17</v>
+        <v>155</v>
       </c>
       <c r="AM16" t="s">
-        <v>22</v>
+        <v>157</v>
       </c>
       <c r="AN16" t="s">
-        <v>18</v>
+        <v>153</v>
+      </c>
+      <c r="AO16">
+        <v>1</v>
+      </c>
+      <c r="AP16" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ16" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS16" t="s">
+        <v>160</v>
+      </c>
+      <c r="AT16">
+        <v>8941</v>
+      </c>
+      <c r="AU16">
+        <v>0.4132</v>
+      </c>
+      <c r="AV16">
+        <v>2</v>
+      </c>
+      <c r="AW16">
+        <v>0.5015191845349909</v>
       </c>
     </row>
-    <row r="17" spans="1:40">
+    <row r="17" spans="1:49">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="D17" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="E17" s="3">
         <v>45894.32219907407</v>
       </c>
       <c r="F17" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="G17">
         <v>41570</v>
@@ -3248,13 +3292,13 @@
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="L17" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="N17" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="O17">
         <v>384.52</v>
@@ -3263,64 +3307,91 @@
         <v>72</v>
       </c>
       <c r="R17" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="S17" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="T17" s="3">
         <v>45894</v>
       </c>
       <c r="U17" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="V17">
         <v>41570</v>
       </c>
       <c r="W17" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="X17">
         <v>384.52</v>
       </c>
       <c r="Y17" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="Z17" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="AA17" s="3">
         <v>45894.56211805555</v>
       </c>
       <c r="AB17" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="AC17" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="AD17" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="AF17" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="AH17" t="s">
-        <v>3</v>
+        <v>109</v>
       </c>
       <c r="AJ17" t="s">
-        <v>2</v>
+        <v>111</v>
       </c>
       <c r="AK17" t="s">
-        <v>8</v>
+        <v>147</v>
       </c>
       <c r="AL17" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="AM17" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="AN17" t="s">
-        <v>20</v>
+        <v>159</v>
+      </c>
+      <c r="AO17">
+        <v>1</v>
+      </c>
+      <c r="AP17" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ17" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR17" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS17" t="s">
+        <v>160</v>
+      </c>
+      <c r="AT17">
+        <v>47976</v>
+      </c>
+      <c r="AU17">
+        <v>0.3992</v>
+      </c>
+      <c r="AV17">
+        <v>0</v>
+      </c>
+      <c r="AW17">
+        <v>0.3537179988803212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update employer branding section
</commit_message>
<xml_diff>
--- a/data/agility/exergi_agility.xlsx
+++ b/data/agility/exergi_agility.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Projects\Gijos\EB Scraping\Dashboard\data\agility\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F23AC75-C941-475F-9502-AC6B0559CEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="141">
   <si>
     <t>Article</t>
   </si>
@@ -163,9 +169,6 @@
     <t>BMQ</t>
   </si>
   <si>
-    <t>Cramo först in och sist ut när Beccs Stockholm växer fram</t>
-  </si>
-  <si>
     <t>Sigholm förbättrar Stockholms energisystem</t>
   </si>
   <si>
@@ -175,9 +178,6 @@
     <t>Skulle lösa klimatkrisen – nu ifrågasätts effekten</t>
   </si>
   <si>
-    <t>Läckta handlingar visar: så kan Sveriges klimatmål förändras</t>
-  </si>
-  <si>
     <t>Pressmeddelande</t>
   </si>
   <si>
@@ -199,9 +199,6 @@
     <t>World's first commercial CO2 'graveyard' opens in Norway</t>
   </si>
   <si>
-    <t>https://www.mynewsdesk.com/se/cramosverige/news/cramo-foerst-in-och-sist-ut-naer-beccs-stockholm-vaexer-fram-501964</t>
-  </si>
-  <si>
     <t>https://www.mynewsdesk.com/se/sigholm-ab/news/sigholm-foerbaettrar-stockholms-energisystem-502356</t>
   </si>
   <si>
@@ -211,9 +208,6 @@
     <t>https://www.svd.se/a/KMoBQy/bakslag-for-koldioxidinlagring-effekten-ifragasatt-i-ny-rapport</t>
   </si>
   <si>
-    <t>https://www.dn.se/sverige/utkast-visar-sa-kan-sveriges-klimatmal-forandras/</t>
-  </si>
-  <si>
     <t>https://www.di.se/bors/pressmeddelande/37245ac1-151c-5f01-ba71-cca6c4df2503/</t>
   </si>
   <si>
@@ -223,9 +217,6 @@
     <t>https://www.kth.se/om/nyheter/centrala-nyheter/kth-leder-nytt-centrum-for-fossilfri-kemikalieproduktion-1.1421672</t>
   </si>
   <si>
-    <t>https://nyheter24.se/nyheter/ekonomi/1416048-prishojningar-lyfter-fjarrvarmejattens-vinst</t>
-  </si>
-  <si>
     <t>https://www.di.se/bors/pressmeddelande/282d4973-b6a7-58f7-b14d-f9127853e82b/</t>
   </si>
   <si>
@@ -247,9 +238,6 @@
     <t>https://www.thelocal.no/20250825/worlds-first-commercial-co2-graveyard-opens-in-norway</t>
   </si>
   <si>
-    <t>Ola Rantatalo</t>
-  </si>
-  <si>
     <t>Viktor Strandgren</t>
   </si>
   <si>
@@ -259,21 +247,12 @@
     <t>Mikael Törnwall</t>
   </si>
   <si>
-    <t>Peter Alestig</t>
-  </si>
-  <si>
-    <t>TT Nyhetsbyrån</t>
-  </si>
-  <si>
     <t>Mynewsdesk</t>
   </si>
   <si>
     <t>Svenska Dagbladet</t>
   </si>
   <si>
-    <t>Dagens Nyheter</t>
-  </si>
-  <si>
     <t>Dagens Industri</t>
   </si>
   <si>
@@ -283,9 +262,6 @@
     <t>kth.se</t>
   </si>
   <si>
-    <t>Nyheter24</t>
-  </si>
-  <si>
     <t>TV4 (Sweden)</t>
   </si>
   <si>
@@ -298,10 +274,6 @@
     <t>The Local (Norway)</t>
   </si>
   <si>
-    <t>Cramo står för byggetableringen när Stockholm Exergis nya anläggning för koldioxidinfångning – Beccs Stockholm – växer fram i Värtahamnen. Johan Gromell, projektledare på Cramo, ser fram emot att stötta den unika satsningen under hela byggtiden. … Han är stolt över att Stockholm Exergi återigen väljer att ge Cramo en nyckelroll i ett spännande projekt:
-–Byggetableringen är ju en grundförutsättning för att alla entreprenörer ska kunna göra sina jobb. Det innebär att vi är först in och sist därifrån.</t>
-  </si>
-  <si>
     <t>Implementeringen innebär att AbS tas i drift både på Stockholm Exergis anläggningar samt deras produktionssamarbetspartners i Stockholmsområdet, där bland annat Norrenergi och Söderenergi ingår. … Om det varit komplext att produktionsoptimera vårt system tidigare så flyttar vi nu gränserna när vi ser på hela staden, säger Per Ljung, Direktör Produktion, Stockholm Exergi.</t>
   </si>
   <si>
@@ -309,10 +281,6 @@
   </si>
   <si>
     <t>Energiföretaget Stockholm Exergi investerar miljardbelopp i en anläggning som ska fånga in miljontals ton koldioxid, som sedan ska lagras djupt under havet i Nordsjön utanför Norges kust.</t>
-  </si>
-  <si>
-    <t>Stockholm Exergi beviljades nyligen 20 miljarder i statligt stöd för en satsning på tekniken vid Värtaverket i Stockholm.
-Även klimatinvesteringar utomlands ska få användas för att nå de svenska klimatmålen, enligt utkastet.</t>
   </si>
   <si>
     <t>Capsol's technology is already licensed for three bio-CCS projects, including Stockholm Exergi's 800,000 tonne-per-year BECCS plant, which reached final investment decision in March 2025, underscoring market traction.</t>
@@ -337,11 +305,6 @@
  EnergiForsk</t>
   </si>
   <si>
-    <t>Nyheter /Ekonomi /Stockholm 
-Publicerad: 28 aug. 2025, kl. 11:44
-Fjärrvärmejätten Stockholm Exergi gjorde en rörelsevinst på en dryg miljard kronor första halvåret, vilket kan jämföras med vinsten på nästan 400 miljoner kronor samma period i fjol.</t>
-  </si>
-  <si>
     <t>It follows the final investment decision at the world's first full-scale plant Stockholm Exergi earlier this year, where our technology is now moving into construction.</t>
   </si>
   <si>
@@ -379,13 +342,7 @@
     <t>Göteborg</t>
   </si>
   <si>
-    <t>Stockholms Lan</t>
-  </si>
-  <si>
     <t>Stockholms län</t>
-  </si>
-  <si>
-    <t>Stockholms län [SE-01]</t>
   </si>
   <si>
     <t>Sweden</t>
@@ -715,13 +672,7 @@
     <t>effekten ifrågasatt i ny rapport</t>
   </si>
   <si>
-    <t>Utkast visar: Så kan Sveriges klimatmål förändras</t>
-  </si>
-  <si>
     <t>KTH leder nytt centrum för fossilfri kemikalieproduktion</t>
-  </si>
-  <si>
-    <t>It seems there was no news article provided. Please share a news article or its content, and I will extract the key topics and assess their sentiment for you.</t>
   </si>
   <si>
     <t>Topic 1: Samarbete mellan Sigholm och Stockholm Exergi
@@ -748,9 +699,6 @@
 Sentiment 3: Positive</t>
   </si>
   <si>
-    <t>It seems there was no news article provided. Please share a news article or text for me to analyze, and I will extract the key topics and assess their sentiment accordingly.</t>
-  </si>
-  <si>
     <t>Topic 1: Inloggning på di.se
 Sentiment 1: Neutral
 Topic 2: Skapa konto utan kostnad
@@ -807,9 +755,6 @@
 Sentiment 3: Negative  </t>
   </si>
   <si>
-    <t>Parsing Error</t>
-  </si>
-  <si>
     <t>The Technologist</t>
   </si>
   <si>
@@ -820,9 +765,6 @@
   </si>
   <si>
     <t>The Expert</t>
-  </si>
-  <si>
-    <t>No Topic</t>
   </si>
   <si>
     <t>Technological Development and Implementation</t>
@@ -858,11 +800,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -939,13 +881,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -983,7 +933,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1017,6 +967,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1051,9 +1002,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1226,14 +1178,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AW17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AW14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AD10" sqref="AD10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:49">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1382,39 +1336,48 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:49">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>49</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E2" s="3">
-        <v>45943.08333333334</v>
+        <v>45951.083333333343</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="G2">
         <v>588967</v>
       </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
       <c r="K2" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="L2" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="M2" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="N2" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="O2">
         <v>5447.94</v>
@@ -1426,87 +1389,108 @@
         <v>49</v>
       </c>
       <c r="S2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="T2" s="3">
-        <v>45943</v>
+        <v>45951</v>
       </c>
       <c r="U2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="V2">
         <v>588967</v>
       </c>
       <c r="W2" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="X2">
         <v>5447.94</v>
       </c>
       <c r="Y2" t="s">
-        <v>118</v>
+        <v>103</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>45951.333333333343</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>104</v>
       </c>
       <c r="AD2" t="s">
-        <v>133</v>
+        <v>117</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>97</v>
       </c>
       <c r="AK2" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="AL2" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="AM2" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="AN2" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="AO2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AP2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR2" t="b">
         <v>0</v>
       </c>
       <c r="AS2" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="AT2">
         <v>9270</v>
       </c>
       <c r="AU2">
-        <v>1</v>
+        <v>0.8498</v>
       </c>
       <c r="AV2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AW2">
-        <v>0.3760287583079845</v>
+        <v>0.61932811966756929</v>
       </c>
     </row>
-    <row r="3" spans="1:49">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>50</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E3" s="3">
-        <v>45951.08333333334</v>
+        <v>45939.0625</v>
       </c>
       <c r="F3" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="G3">
         <v>588967</v>
@@ -1521,16 +1505,16 @@
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="L3" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="M3" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="N3" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="O3">
         <v>5447.94</v>
@@ -1542,135 +1526,123 @@
         <v>50</v>
       </c>
       <c r="S3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="T3" s="3">
-        <v>45951</v>
+        <v>45939</v>
       </c>
       <c r="U3" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="V3">
         <v>588967</v>
       </c>
       <c r="W3" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="X3">
         <v>5447.94</v>
       </c>
       <c r="Y3" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>45939.3125</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD3" t="s">
         <v>118</v>
       </c>
-      <c r="Z3" t="s">
-        <v>119</v>
-      </c>
-      <c r="AA3" s="3">
-        <v>45951.33333333334</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>119</v>
-      </c>
-      <c r="AD3" t="s">
+      <c r="AF3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>128</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>132</v>
+      </c>
+      <c r="AM3" t="s">
         <v>134</v>
       </c>
-      <c r="AF3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>146</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>151</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>155</v>
-      </c>
       <c r="AN3" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="AO3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AP3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR3" t="b">
         <v>0</v>
       </c>
       <c r="AS3" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="AT3">
         <v>9270</v>
       </c>
       <c r="AU3">
-        <v>0.8498</v>
+        <v>0.76200000000000001</v>
       </c>
       <c r="AV3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AW3">
-        <v>0.6193281196675693</v>
+        <v>0.37602875830798449</v>
       </c>
     </row>
-    <row r="4" spans="1:49">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>51</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E4" s="3">
-        <v>45939.0625</v>
+        <v>45908.484363425923</v>
       </c>
       <c r="F4" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="G4">
-        <v>588967</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
+        <v>2285700</v>
       </c>
       <c r="K4" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="L4" t="s">
-        <v>112</v>
-      </c>
-      <c r="M4" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="N4" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="O4">
-        <v>5447.94</v>
+        <v>21142.720000000001</v>
       </c>
       <c r="P4">
         <v>89</v>
@@ -1679,299 +1651,323 @@
         <v>51</v>
       </c>
       <c r="S4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="T4" s="3">
-        <v>45939</v>
+        <v>45908</v>
       </c>
       <c r="U4" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="V4">
-        <v>588967</v>
+        <v>2285700</v>
       </c>
       <c r="W4" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="X4">
-        <v>5447.94</v>
+        <v>21142.720000000001</v>
       </c>
       <c r="Y4" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="Z4" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="AA4" s="3">
-        <v>45939.3125</v>
+        <v>45908.648923611108</v>
       </c>
       <c r="AB4" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="AC4" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="AD4" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="AF4" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="AH4" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="AJ4" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="AK4" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="AL4" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="AM4" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="AN4" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="AO4">
         <v>1</v>
       </c>
       <c r="AP4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR4" t="b">
         <v>0</v>
       </c>
       <c r="AS4" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="AT4">
-        <v>9270</v>
+        <v>8941</v>
       </c>
       <c r="AU4">
-        <v>0.762</v>
+        <v>0.69959999999999989</v>
       </c>
       <c r="AV4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AW4">
-        <v>0.3760287583079845</v>
+        <v>0.50151918453499089</v>
       </c>
     </row>
-    <row r="5" spans="1:49">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>52</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E5" s="3">
-        <v>45908.48436342592</v>
+        <v>45908</v>
       </c>
       <c r="F5" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G5">
-        <v>2285700</v>
+        <v>1098249</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="L5" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="N5" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="O5">
-        <v>21142.72</v>
+        <v>10158.799999999999</v>
       </c>
       <c r="P5">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="R5" t="s">
         <v>52</v>
       </c>
       <c r="S5" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="T5" s="3">
         <v>45908</v>
       </c>
       <c r="U5" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="V5">
-        <v>2285700</v>
+        <v>1098249</v>
       </c>
       <c r="W5" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="X5">
-        <v>21142.72</v>
+        <v>10158.799999999999</v>
       </c>
       <c r="Y5" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="Z5" t="s">
-        <v>121</v>
-      </c>
-      <c r="AA5" s="3">
-        <v>45908.64892361111</v>
+        <v>107</v>
       </c>
       <c r="AB5" t="s">
-        <v>130</v>
+        <v>52</v>
       </c>
       <c r="AC5" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="AD5" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="AF5" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="AH5" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="AJ5" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="AK5" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="AL5" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="AM5" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="AN5" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="AO5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR5" t="b">
         <v>0</v>
       </c>
       <c r="AS5" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="AT5">
-        <v>8941</v>
+        <v>9130</v>
       </c>
       <c r="AU5">
-        <v>0.6995999999999999</v>
+        <v>0.61180000000000001</v>
       </c>
       <c r="AV5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AW5">
-        <v>0.5015191845349909</v>
+        <v>0.37623528820205321</v>
       </c>
     </row>
-    <row r="6" spans="1:49">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>53</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E6" s="3">
-        <v>45910.14776620371</v>
+        <v>45905.201967592591</v>
       </c>
       <c r="F6" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="G6">
-        <v>1769848</v>
+        <v>3773492</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="L6" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="M6" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="N6" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="O6">
-        <v>16371.09</v>
+        <v>34904.800000000003</v>
       </c>
       <c r="P6">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="R6" t="s">
         <v>53</v>
       </c>
       <c r="S6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="T6" s="3">
-        <v>45910</v>
+        <v>45905</v>
       </c>
       <c r="U6" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="V6">
-        <v>1769848</v>
+        <v>3773492</v>
       </c>
       <c r="W6" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="X6">
-        <v>16371.09</v>
+        <v>34904.800000000003</v>
       </c>
       <c r="Y6" t="s">
-        <v>118</v>
+        <v>103</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>108</v>
       </c>
       <c r="AA6" s="3">
-        <v>45910.39491898148</v>
+        <v>45905.451967592591</v>
       </c>
       <c r="AB6" t="s">
-        <v>131</v>
+        <v>53</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>108</v>
       </c>
       <c r="AD6" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>97</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>128</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>134</v>
+      </c>
+      <c r="AM6" t="s">
         <v>137</v>
       </c>
-      <c r="AK6" t="s">
-        <v>145</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>150</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>150</v>
-      </c>
       <c r="AN6" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="AO6">
         <v>0</v>
@@ -1986,39 +1982,39 @@
         <v>0</v>
       </c>
       <c r="AS6" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="AT6">
-        <v>9583</v>
+        <v>3300</v>
       </c>
       <c r="AU6">
-        <v>0.6513</v>
+        <v>0.57840000000000003</v>
       </c>
       <c r="AV6">
         <v>0</v>
       </c>
       <c r="AW6">
-        <v>0.3755780784953673</v>
+        <v>0.390046439378816</v>
       </c>
     </row>
-    <row r="7" spans="1:49">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>54</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E7" s="3">
-        <v>45908</v>
+        <v>45903</v>
       </c>
       <c r="F7" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="G7">
-        <v>1098249</v>
+        <v>562175</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -2030,570 +2026,579 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>109</v>
-      </c>
-      <c r="L7" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="N7" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="O7">
-        <v>10158.8</v>
+        <v>5200.12</v>
       </c>
       <c r="P7">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="R7" t="s">
         <v>54</v>
       </c>
       <c r="S7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="T7" s="3">
-        <v>45908</v>
+        <v>45903</v>
       </c>
       <c r="U7" t="s">
+        <v>89</v>
+      </c>
+      <c r="V7">
+        <v>562175</v>
+      </c>
+      <c r="W7" t="s">
+        <v>102</v>
+      </c>
+      <c r="X7">
+        <v>5200.12</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>45973</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>122</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>97</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>128</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>133</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AO7">
+        <v>0</v>
+      </c>
+      <c r="AP7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>140</v>
+      </c>
+      <c r="AT7">
+        <v>12526</v>
+      </c>
+      <c r="AU7">
+        <v>0.5494</v>
+      </c>
+      <c r="AV7">
+        <v>0</v>
+      </c>
+      <c r="AW7">
+        <v>0.37194336226983471</v>
+      </c>
+    </row>
+    <row r="8" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="3">
+        <v>45898</v>
+      </c>
+      <c r="F8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8">
+        <v>1098249</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L8" t="s">
         <v>99</v>
       </c>
-      <c r="V7">
+      <c r="N8" t="s">
+        <v>102</v>
+      </c>
+      <c r="O8">
+        <v>10158.799999999999</v>
+      </c>
+      <c r="P8">
+        <v>70</v>
+      </c>
+      <c r="R8" t="s">
+        <v>52</v>
+      </c>
+      <c r="S8" t="s">
+        <v>77</v>
+      </c>
+      <c r="T8" s="3">
+        <v>45898</v>
+      </c>
+      <c r="U8" t="s">
+        <v>90</v>
+      </c>
+      <c r="V8">
         <v>1098249</v>
       </c>
-      <c r="W7" t="s">
-        <v>117</v>
-      </c>
-      <c r="X7">
-        <v>10158.8</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>118</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>122</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>122</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>138</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>109</v>
-      </c>
-      <c r="AH7" t="s">
+      <c r="W8" t="s">
+        <v>102</v>
+      </c>
+      <c r="X8">
+        <v>10158.799999999999</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>129</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>134</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>134</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>135</v>
+      </c>
+      <c r="AO8">
+        <v>0</v>
+      </c>
+      <c r="AP8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>140</v>
+      </c>
+      <c r="AT8">
+        <v>9130</v>
+      </c>
+      <c r="AU8">
+        <v>0.50109999999999999</v>
+      </c>
+      <c r="AV8">
+        <v>0</v>
+      </c>
+      <c r="AW8">
+        <v>0.37623528820205321</v>
+      </c>
+    </row>
+    <row r="9" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="3">
+        <v>45897.240219907413</v>
+      </c>
+      <c r="F9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9">
+        <v>1191791</v>
+      </c>
+      <c r="K9" t="s">
+        <v>97</v>
+      </c>
+      <c r="M9" t="s">
+        <v>101</v>
+      </c>
+      <c r="N9" t="s">
+        <v>102</v>
+      </c>
+      <c r="O9">
+        <v>11024.07</v>
+      </c>
+      <c r="P9">
+        <v>69</v>
+      </c>
+      <c r="R9" t="s">
+        <v>55</v>
+      </c>
+      <c r="S9" t="s">
+        <v>80</v>
+      </c>
+      <c r="T9" s="3">
+        <v>45897</v>
+      </c>
+      <c r="U9" t="s">
+        <v>91</v>
+      </c>
+      <c r="V9">
+        <v>1191791</v>
+      </c>
+      <c r="W9" t="s">
+        <v>102</v>
+      </c>
+      <c r="X9">
+        <v>11024.07</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z9" t="s">
         <v>110</v>
       </c>
-      <c r="AJ7" t="s">
+      <c r="AA9" s="3">
+        <v>45897.405092592591</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC9" t="s">
         <v>110</v>
       </c>
-      <c r="AK7" t="s">
-        <v>148</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>154</v>
-      </c>
-      <c r="AM7" t="s">
-        <v>154</v>
-      </c>
-      <c r="AN7" t="s">
-        <v>155</v>
-      </c>
-      <c r="AO7">
-        <v>0</v>
-      </c>
-      <c r="AP7" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ7" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR7" t="b">
-        <v>0</v>
-      </c>
-      <c r="AS7" t="s">
-        <v>160</v>
-      </c>
-      <c r="AT7">
-        <v>9130</v>
-      </c>
-      <c r="AU7">
-        <v>0.6118</v>
-      </c>
-      <c r="AV7">
-        <v>0</v>
-      </c>
-      <c r="AW7">
-        <v>0.3762352882020532</v>
+      <c r="AD9" t="s">
+        <v>123</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>130</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>136</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>136</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>136</v>
+      </c>
+      <c r="AO9">
+        <v>1</v>
+      </c>
+      <c r="AP9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>140</v>
+      </c>
+      <c r="AT9">
+        <v>34677</v>
+      </c>
+      <c r="AU9">
+        <v>0.48039999999999999</v>
+      </c>
+      <c r="AV9">
+        <v>2</v>
+      </c>
+      <c r="AW9">
+        <v>0.48312370254836479</v>
       </c>
     </row>
-    <row r="8" spans="1:49">
-      <c r="A8" t="s">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E8" s="3">
-        <v>45905.20196759259</v>
-      </c>
-      <c r="F8" t="s">
-        <v>100</v>
-      </c>
-      <c r="G8">
-        <v>3773492</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8" t="s">
-        <v>110</v>
-      </c>
-      <c r="L8" t="s">
-        <v>112</v>
-      </c>
-      <c r="M8" t="s">
-        <v>115</v>
-      </c>
-      <c r="N8" t="s">
-        <v>117</v>
-      </c>
-      <c r="O8">
-        <v>34904.8</v>
-      </c>
-      <c r="P8">
-        <v>84</v>
-      </c>
-      <c r="R8" t="s">
+      <c r="D10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="3">
+        <v>45897.238518518519</v>
+      </c>
+      <c r="F10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G10">
+        <v>4648460</v>
+      </c>
+      <c r="K10" t="s">
+        <v>97</v>
+      </c>
+      <c r="N10" t="s">
+        <v>102</v>
+      </c>
+      <c r="O10">
+        <v>42998.26</v>
+      </c>
+      <c r="P10">
+        <v>90</v>
+      </c>
+      <c r="R10" t="s">
         <v>55</v>
       </c>
-      <c r="S8" t="s">
-        <v>87</v>
-      </c>
-      <c r="T8" s="3">
-        <v>45905</v>
-      </c>
-      <c r="U8" t="s">
-        <v>100</v>
-      </c>
-      <c r="V8">
-        <v>3773492</v>
-      </c>
-      <c r="W8" t="s">
-        <v>117</v>
-      </c>
-      <c r="X8">
-        <v>34904.8</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>118</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA8" s="3">
-        <v>45905.45196759259</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>123</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>139</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>110</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>110</v>
-      </c>
-      <c r="AK8" t="s">
-        <v>147</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>154</v>
-      </c>
-      <c r="AM8" t="s">
-        <v>157</v>
-      </c>
-      <c r="AN8" t="s">
-        <v>152</v>
-      </c>
-      <c r="AO8">
-        <v>0</v>
-      </c>
-      <c r="AP8" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ8" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR8" t="b">
-        <v>0</v>
-      </c>
-      <c r="AS8" t="s">
-        <v>160</v>
-      </c>
-      <c r="AT8">
-        <v>3300</v>
-      </c>
-      <c r="AU8">
-        <v>0.5784</v>
-      </c>
-      <c r="AV8">
-        <v>0</v>
-      </c>
-      <c r="AW8">
-        <v>0.390046439378816</v>
-      </c>
-    </row>
-    <row r="9" spans="1:49">
-      <c r="A9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" t="s">
-        <v>88</v>
-      </c>
-      <c r="E9" s="3">
-        <v>45903</v>
-      </c>
-      <c r="F9" t="s">
-        <v>101</v>
-      </c>
-      <c r="G9">
-        <v>562175</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9" t="s">
-        <v>110</v>
-      </c>
-      <c r="N9" t="s">
-        <v>117</v>
-      </c>
-      <c r="O9">
-        <v>5200.12</v>
-      </c>
-      <c r="P9">
-        <v>75</v>
-      </c>
-      <c r="R9" t="s">
-        <v>56</v>
-      </c>
-      <c r="S9" t="s">
-        <v>88</v>
-      </c>
-      <c r="T9" s="3">
-        <v>45903</v>
-      </c>
-      <c r="U9" t="s">
-        <v>101</v>
-      </c>
-      <c r="V9">
-        <v>562175</v>
-      </c>
-      <c r="W9" t="s">
-        <v>117</v>
-      </c>
-      <c r="X9">
-        <v>5200.12</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>118</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>124</v>
-      </c>
-      <c r="AA9" s="3">
-        <v>45973</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>132</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>124</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>140</v>
-      </c>
-      <c r="AF9" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>110</v>
-      </c>
-      <c r="AJ9" t="s">
-        <v>110</v>
-      </c>
-      <c r="AK9" t="s">
-        <v>147</v>
-      </c>
-      <c r="AL9" t="s">
-        <v>155</v>
-      </c>
-      <c r="AM9" t="s">
-        <v>153</v>
-      </c>
-      <c r="AN9" t="s">
-        <v>159</v>
-      </c>
-      <c r="AO9">
-        <v>0</v>
-      </c>
-      <c r="AP9" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ9" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR9" t="b">
-        <v>0</v>
-      </c>
-      <c r="AS9" t="s">
-        <v>160</v>
-      </c>
-      <c r="AT9">
-        <v>12526</v>
-      </c>
-      <c r="AU9">
-        <v>0.5494</v>
-      </c>
-      <c r="AV9">
-        <v>0</v>
-      </c>
-      <c r="AW9">
-        <v>0.3719433622698347</v>
-      </c>
-    </row>
-    <row r="10" spans="1:49">
-      <c r="A10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E10" s="3">
-        <v>45897.23893518518</v>
-      </c>
-      <c r="F10" t="s">
-        <v>102</v>
-      </c>
-      <c r="G10">
-        <v>778729</v>
-      </c>
-      <c r="K10" t="s">
-        <v>109</v>
-      </c>
-      <c r="M10" t="s">
-        <v>116</v>
-      </c>
-      <c r="N10" t="s">
-        <v>117</v>
-      </c>
-      <c r="O10">
-        <v>7203.24</v>
-      </c>
-      <c r="P10">
-        <v>68</v>
-      </c>
-      <c r="R10" t="s">
-        <v>57</v>
-      </c>
       <c r="S10" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="T10" s="3">
         <v>45897</v>
       </c>
       <c r="U10" t="s">
+        <v>92</v>
+      </c>
+      <c r="V10">
+        <v>4648460</v>
+      </c>
+      <c r="W10" t="s">
         <v>102</v>
       </c>
-      <c r="V10">
-        <v>778729</v>
-      </c>
-      <c r="W10" t="s">
-        <v>117</v>
-      </c>
       <c r="X10">
-        <v>7203.24</v>
+        <v>42998.26</v>
       </c>
       <c r="Y10" t="s">
-        <v>118</v>
+        <v>103</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>45897.405185185176</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>110</v>
       </c>
       <c r="AD10" t="s">
-        <v>133</v>
+        <v>123</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>98</v>
       </c>
       <c r="AK10" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="AL10" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="AM10" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="AN10" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="AO10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR10" t="b">
         <v>0</v>
       </c>
       <c r="AS10" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="AT10">
-        <v>50866</v>
+        <v>14771</v>
       </c>
       <c r="AU10">
-        <v>0.5239</v>
+        <v>0.46160000000000001</v>
       </c>
       <c r="AV10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AW10">
-        <v>0.3529241379084694</v>
+        <v>0.49470594068310308</v>
       </c>
     </row>
-    <row r="11" spans="1:49">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E11" s="3">
-        <v>45898</v>
+        <v>45897.183287037027</v>
       </c>
       <c r="F11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11">
+        <v>3773492</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>97</v>
+      </c>
+      <c r="L11" t="s">
+        <v>99</v>
+      </c>
+      <c r="M11" t="s">
+        <v>101</v>
+      </c>
+      <c r="N11" t="s">
+        <v>102</v>
+      </c>
+      <c r="O11">
+        <v>34904.800000000003</v>
+      </c>
+      <c r="P11">
+        <v>84</v>
+      </c>
+      <c r="R11" t="s">
+        <v>56</v>
+      </c>
+      <c r="S11" t="s">
+        <v>78</v>
+      </c>
+      <c r="T11" s="3">
+        <v>45897</v>
+      </c>
+      <c r="U11" t="s">
+        <v>88</v>
+      </c>
+      <c r="V11">
+        <v>3773492</v>
+      </c>
+      <c r="W11" t="s">
+        <v>102</v>
+      </c>
+      <c r="X11">
+        <v>34904.800000000003</v>
+      </c>
+      <c r="Y11" t="s">
         <v>103</v>
       </c>
-      <c r="G11">
-        <v>1098249</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11" t="s">
-        <v>109</v>
-      </c>
-      <c r="L11" t="s">
-        <v>112</v>
-      </c>
-      <c r="N11" t="s">
-        <v>117</v>
-      </c>
-      <c r="O11">
-        <v>10158.8</v>
-      </c>
-      <c r="P11">
-        <v>70</v>
-      </c>
-      <c r="R11" t="s">
-        <v>54</v>
-      </c>
-      <c r="S11" t="s">
-        <v>86</v>
-      </c>
-      <c r="T11" s="3">
-        <v>45898</v>
-      </c>
-      <c r="U11" t="s">
-        <v>103</v>
-      </c>
-      <c r="V11">
-        <v>1098249</v>
-      </c>
-      <c r="W11" t="s">
-        <v>117</v>
-      </c>
-      <c r="X11">
-        <v>10158.8</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>118</v>
-      </c>
       <c r="Z11" t="s">
-        <v>122</v>
+        <v>111</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>45897.433287037027</v>
       </c>
       <c r="AB11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AC11" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="AD11" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="AF11" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="AH11" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="AJ11" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="AK11" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="AL11" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="AM11" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="AN11" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="AO11">
         <v>0</v>
@@ -2608,114 +2613,123 @@
         <v>0</v>
       </c>
       <c r="AS11" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="AT11">
-        <v>9130</v>
+        <v>3300</v>
       </c>
       <c r="AU11">
-        <v>0.5011</v>
+        <v>0.44419999999999998</v>
       </c>
       <c r="AV11">
         <v>0</v>
       </c>
       <c r="AW11">
-        <v>0.3762352882020532</v>
+        <v>0.390046439378816</v>
       </c>
     </row>
-    <row r="12" spans="1:49">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="E12" s="3">
-        <v>45897.24021990741</v>
+        <v>45897.238379629627</v>
       </c>
       <c r="F12" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="G12">
-        <v>1191791</v>
+        <v>1594618</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>110</v>
-      </c>
-      <c r="M12" t="s">
-        <v>115</v>
+        <v>97</v>
+      </c>
+      <c r="L12" t="s">
+        <v>100</v>
       </c>
       <c r="N12" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="O12">
-        <v>11024.07</v>
+        <v>14750.22</v>
       </c>
       <c r="P12">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="R12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="S12" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="T12" s="3">
         <v>45897</v>
       </c>
       <c r="U12" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="V12">
-        <v>1191791</v>
+        <v>1594618</v>
       </c>
       <c r="W12" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="X12">
-        <v>11024.07</v>
+        <v>14750.22</v>
       </c>
       <c r="Y12" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="Z12" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="AA12" s="3">
-        <v>45897.40509259259</v>
+        <v>45897.405046296299</v>
       </c>
       <c r="AB12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AC12" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="AD12" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="AF12" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="AH12" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="AJ12" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="AK12" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="AL12" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="AM12" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="AN12" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="AO12">
         <v>1</v>
@@ -2730,111 +2744,126 @@
         <v>0</v>
       </c>
       <c r="AS12" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="AT12">
-        <v>34677</v>
+        <v>18918</v>
       </c>
       <c r="AU12">
-        <v>0.4804</v>
+        <v>0.42820000000000003</v>
       </c>
       <c r="AV12">
         <v>2</v>
       </c>
       <c r="AW12">
-        <v>0.4831237025483648</v>
+        <v>0.49134764933963909</v>
       </c>
     </row>
-    <row r="13" spans="1:49">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>57</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
+      </c>
+      <c r="C13" t="s">
+        <v>74</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="E13" s="3">
-        <v>45897.23851851852</v>
+        <v>45892.464143518519</v>
       </c>
       <c r="F13" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="G13">
-        <v>4648460</v>
+        <v>2285700</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>110</v>
+        <v>97</v>
+      </c>
+      <c r="L13" t="s">
+        <v>99</v>
       </c>
       <c r="N13" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="O13">
-        <v>42998.26</v>
+        <v>21142.720000000001</v>
       </c>
       <c r="P13">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R13" t="s">
         <v>57</v>
       </c>
       <c r="S13" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="T13" s="3">
-        <v>45897</v>
+        <v>45892</v>
       </c>
       <c r="U13" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="V13">
-        <v>4648460</v>
+        <v>2285700</v>
       </c>
       <c r="W13" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="X13">
-        <v>42998.26</v>
+        <v>21142.720000000001</v>
       </c>
       <c r="Y13" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="Z13" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="AA13" s="3">
-        <v>45897.40518518518</v>
+        <v>45892.623310185183</v>
       </c>
       <c r="AB13" t="s">
         <v>57</v>
       </c>
       <c r="AC13" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD13" t="s">
         <v>125</v>
       </c>
-      <c r="AD13" t="s">
-        <v>141</v>
-      </c>
       <c r="AF13" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="AH13" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="AJ13" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="AK13" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="AL13" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="AM13" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="AN13" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
       <c r="AO13">
         <v>1</v>
@@ -2849,39 +2878,39 @@
         <v>0</v>
       </c>
       <c r="AS13" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="AT13">
-        <v>14771</v>
+        <v>8941</v>
       </c>
       <c r="AU13">
-        <v>0.4616</v>
+        <v>0.41320000000000001</v>
       </c>
       <c r="AV13">
         <v>2</v>
       </c>
       <c r="AW13">
-        <v>0.4947059406831031</v>
+        <v>0.50151918453499089</v>
       </c>
     </row>
-    <row r="14" spans="1:49">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>58</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D14" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E14" s="3">
-        <v>45897.18328703703</v>
+        <v>45894.322199074071</v>
       </c>
       <c r="F14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G14">
-        <v>3773492</v>
+        <v>41570</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -2893,85 +2922,82 @@
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="L14" t="s">
-        <v>112</v>
-      </c>
-      <c r="M14" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="N14" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="O14">
-        <v>34904.8</v>
+        <v>384.52</v>
       </c>
       <c r="P14">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="R14" t="s">
         <v>58</v>
       </c>
       <c r="S14" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="T14" s="3">
-        <v>45897</v>
+        <v>45894</v>
       </c>
       <c r="U14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="V14">
-        <v>3773492</v>
+        <v>41570</v>
       </c>
       <c r="W14" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="X14">
-        <v>34904.8</v>
+        <v>384.52</v>
       </c>
       <c r="Y14" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="Z14" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="AA14" s="3">
-        <v>45897.43328703703</v>
+        <v>45894.562118055554</v>
       </c>
       <c r="AB14" t="s">
         <v>58</v>
       </c>
       <c r="AC14" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD14" t="s">
         <v>126</v>
       </c>
-      <c r="AD14" t="s">
-        <v>142</v>
-      </c>
       <c r="AF14" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="AH14" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="AJ14" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="AK14" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="AL14" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="AM14" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="AN14" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="AO14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP14" t="b">
         <v>0</v>
@@ -2983,435 +3009,36 @@
         <v>0</v>
       </c>
       <c r="AS14" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="AT14">
-        <v>3300</v>
+        <v>47976</v>
       </c>
       <c r="AU14">
-        <v>0.4442</v>
+        <v>0.3992</v>
       </c>
       <c r="AV14">
         <v>0</v>
       </c>
       <c r="AW14">
-        <v>0.390046439378816</v>
-      </c>
-    </row>
-    <row r="15" spans="1:49">
-      <c r="A15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" t="s">
-        <v>92</v>
-      </c>
-      <c r="E15" s="3">
-        <v>45897.23837962963</v>
-      </c>
-      <c r="F15" t="s">
-        <v>106</v>
-      </c>
-      <c r="G15">
-        <v>1594618</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15" t="s">
-        <v>110</v>
-      </c>
-      <c r="L15" t="s">
-        <v>113</v>
-      </c>
-      <c r="N15" t="s">
-        <v>117</v>
-      </c>
-      <c r="O15">
-        <v>14750.22</v>
-      </c>
-      <c r="P15">
-        <v>78</v>
-      </c>
-      <c r="R15" t="s">
-        <v>57</v>
-      </c>
-      <c r="S15" t="s">
-        <v>92</v>
-      </c>
-      <c r="T15" s="3">
-        <v>45897</v>
-      </c>
-      <c r="U15" t="s">
-        <v>106</v>
-      </c>
-      <c r="V15">
-        <v>1594618</v>
-      </c>
-      <c r="W15" t="s">
-        <v>117</v>
-      </c>
-      <c r="X15">
-        <v>14750.22</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>118</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>125</v>
-      </c>
-      <c r="AA15" s="3">
-        <v>45897.4050462963</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC15" t="s">
-        <v>125</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>141</v>
-      </c>
-      <c r="AF15" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH15" t="s">
-        <v>110</v>
-      </c>
-      <c r="AJ15" t="s">
-        <v>111</v>
-      </c>
-      <c r="AK15" t="s">
-        <v>148</v>
-      </c>
-      <c r="AL15" t="s">
-        <v>156</v>
-      </c>
-      <c r="AM15" t="s">
-        <v>156</v>
-      </c>
-      <c r="AN15" t="s">
-        <v>156</v>
-      </c>
-      <c r="AO15">
-        <v>1</v>
-      </c>
-      <c r="AP15" t="b">
-        <v>1</v>
-      </c>
-      <c r="AQ15" t="b">
-        <v>1</v>
-      </c>
-      <c r="AR15" t="b">
-        <v>0</v>
-      </c>
-      <c r="AS15" t="s">
-        <v>160</v>
-      </c>
-      <c r="AT15">
-        <v>18918</v>
-      </c>
-      <c r="AU15">
-        <v>0.4282</v>
-      </c>
-      <c r="AV15">
-        <v>2</v>
-      </c>
-      <c r="AW15">
-        <v>0.4913476493396391</v>
-      </c>
-    </row>
-    <row r="16" spans="1:49">
-      <c r="A16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D16" t="s">
-        <v>84</v>
-      </c>
-      <c r="E16" s="3">
-        <v>45892.46414351852</v>
-      </c>
-      <c r="F16" t="s">
-        <v>107</v>
-      </c>
-      <c r="G16">
-        <v>2285700</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16" t="s">
-        <v>110</v>
-      </c>
-      <c r="L16" t="s">
-        <v>112</v>
-      </c>
-      <c r="N16" t="s">
-        <v>117</v>
-      </c>
-      <c r="O16">
-        <v>21142.72</v>
-      </c>
-      <c r="P16">
-        <v>89</v>
-      </c>
-      <c r="R16" t="s">
-        <v>59</v>
-      </c>
-      <c r="S16" t="s">
-        <v>84</v>
-      </c>
-      <c r="T16" s="3">
-        <v>45892</v>
-      </c>
-      <c r="U16" t="s">
-        <v>107</v>
-      </c>
-      <c r="V16">
-        <v>2285700</v>
-      </c>
-      <c r="W16" t="s">
-        <v>117</v>
-      </c>
-      <c r="X16">
-        <v>21142.72</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>118</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>127</v>
-      </c>
-      <c r="AA16" s="3">
-        <v>45892.62331018518</v>
-      </c>
-      <c r="AB16" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC16" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD16" t="s">
-        <v>143</v>
-      </c>
-      <c r="AF16" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH16" t="s">
-        <v>110</v>
-      </c>
-      <c r="AJ16" t="s">
-        <v>110</v>
-      </c>
-      <c r="AK16" t="s">
-        <v>147</v>
-      </c>
-      <c r="AL16" t="s">
-        <v>155</v>
-      </c>
-      <c r="AM16" t="s">
-        <v>157</v>
-      </c>
-      <c r="AN16" t="s">
-        <v>153</v>
-      </c>
-      <c r="AO16">
-        <v>1</v>
-      </c>
-      <c r="AP16" t="b">
-        <v>1</v>
-      </c>
-      <c r="AQ16" t="b">
-        <v>1</v>
-      </c>
-      <c r="AR16" t="b">
-        <v>0</v>
-      </c>
-      <c r="AS16" t="s">
-        <v>160</v>
-      </c>
-      <c r="AT16">
-        <v>8941</v>
-      </c>
-      <c r="AU16">
-        <v>0.4132</v>
-      </c>
-      <c r="AV16">
-        <v>2</v>
-      </c>
-      <c r="AW16">
-        <v>0.5015191845349909</v>
-      </c>
-    </row>
-    <row r="17" spans="1:49">
-      <c r="A17" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" t="s">
-        <v>93</v>
-      </c>
-      <c r="E17" s="3">
-        <v>45894.32219907407</v>
-      </c>
-      <c r="F17" t="s">
-        <v>108</v>
-      </c>
-      <c r="G17">
-        <v>41570</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17" t="s">
-        <v>110</v>
-      </c>
-      <c r="L17" t="s">
-        <v>112</v>
-      </c>
-      <c r="N17" t="s">
-        <v>117</v>
-      </c>
-      <c r="O17">
-        <v>384.52</v>
-      </c>
-      <c r="P17">
-        <v>72</v>
-      </c>
-      <c r="R17" t="s">
-        <v>60</v>
-      </c>
-      <c r="S17" t="s">
-        <v>93</v>
-      </c>
-      <c r="T17" s="3">
-        <v>45894</v>
-      </c>
-      <c r="U17" t="s">
-        <v>108</v>
-      </c>
-      <c r="V17">
-        <v>41570</v>
-      </c>
-      <c r="W17" t="s">
-        <v>117</v>
-      </c>
-      <c r="X17">
-        <v>384.52</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>118</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>128</v>
-      </c>
-      <c r="AA17" s="3">
-        <v>45894.56211805555</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC17" t="s">
-        <v>128</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>144</v>
-      </c>
-      <c r="AF17" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>109</v>
-      </c>
-      <c r="AJ17" t="s">
-        <v>111</v>
-      </c>
-      <c r="AK17" t="s">
-        <v>147</v>
-      </c>
-      <c r="AL17" t="s">
-        <v>153</v>
-      </c>
-      <c r="AM17" t="s">
-        <v>153</v>
-      </c>
-      <c r="AN17" t="s">
-        <v>159</v>
-      </c>
-      <c r="AO17">
-        <v>1</v>
-      </c>
-      <c r="AP17" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ17" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR17" t="b">
-        <v>0</v>
-      </c>
-      <c r="AS17" t="s">
-        <v>160</v>
-      </c>
-      <c r="AT17">
-        <v>47976</v>
-      </c>
-      <c r="AU17">
-        <v>0.3992</v>
-      </c>
-      <c r="AV17">
-        <v>0</v>
-      </c>
-      <c r="AW17">
-        <v>0.3537179988803212</v>
+        <v>0.35371799888032118</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-    <hyperlink ref="B12" r:id="rId11"/>
-    <hyperlink ref="B13" r:id="rId12"/>
-    <hyperlink ref="B14" r:id="rId13"/>
-    <hyperlink ref="B15" r:id="rId14"/>
-    <hyperlink ref="B16" r:id="rId15"/>
-    <hyperlink ref="B17" r:id="rId16"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>